<commit_message>
Reduce PIP deduction from 40% to 20% in salary page
Updated the PIP deduction logic and all related labels in the salary dashboard to apply a 20% deduction instead of 40% for employees in the PIP department. Also updated the sample Salary Format.xlsx file.
</commit_message>
<xml_diff>
--- a/public/sample/Salary Format.xlsx
+++ b/public/sample/Salary Format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Office\Projects\Automated Salary Maker\public\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38665B13-7246-4C70-A8C9-90B2A4359EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84E782C-7CB5-41BD-BEA0-44A984F2EDC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="71">
   <si>
     <t xml:space="preserve">Week off </t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>WFH</t>
+  </si>
+  <si>
+    <t>SALES (PIP)</t>
   </si>
 </sst>
 </file>
@@ -466,16 +469,16 @@
     <xf numFmtId="20" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="7" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -976,9 +979,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F44" sqref="F44"/>
+      <selection pane="topRight" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1263,7 +1266,7 @@
       <c r="L4" s="10">
         <v>9.5500001907348633</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N4" s="10">
@@ -1275,10 +1278,10 @@
       <c r="P4" s="10">
         <v>9.5</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="R4" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S4" s="19" t="s">
@@ -1293,7 +1296,7 @@
       <c r="V4" s="10">
         <v>10</v>
       </c>
-      <c r="W4" s="21" t="s">
+      <c r="W4" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X4" s="10">
@@ -1305,7 +1308,7 @@
       <c r="Z4" s="10">
         <v>9.4799995422363281</v>
       </c>
-      <c r="AA4" s="20" t="s">
+      <c r="AA4" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB4" s="10">
@@ -1326,7 +1329,7 @@
       <c r="AG4" s="10">
         <v>10</v>
       </c>
-      <c r="AH4" s="20" t="s">
+      <c r="AH4" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI4" s="19" t="s">
@@ -1367,7 +1370,7 @@
       <c r="L5" s="10">
         <v>18.389999389648438</v>
       </c>
-      <c r="M5" s="20"/>
+      <c r="M5" s="23"/>
       <c r="N5" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -1377,8 +1380,8 @@
       <c r="P5" s="10">
         <v>14.050000190734863</v>
       </c>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="20"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="23"/>
       <c r="S5" s="19"/>
       <c r="T5" s="10">
         <v>18.32</v>
@@ -1389,7 +1392,7 @@
       <c r="V5" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="W5" s="21"/>
+      <c r="W5" s="22"/>
       <c r="X5" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -1399,7 +1402,7 @@
       <c r="Z5" s="10">
         <v>18.319999694824219</v>
       </c>
-      <c r="AA5" s="20"/>
+      <c r="AA5" s="23"/>
       <c r="AB5" s="10">
         <v>18.329999999999998</v>
       </c>
@@ -1418,7 +1421,7 @@
       <c r="AG5" s="10">
         <v>18.32</v>
       </c>
-      <c r="AH5" s="20"/>
+      <c r="AH5" s="23"/>
       <c r="AI5" s="19"/>
       <c r="AJ5" s="19"/>
       <c r="AK5" s="19"/>
@@ -1480,7 +1483,7 @@
       <c r="P7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="Q7" s="21" t="s">
+      <c r="Q7" s="22" t="s">
         <v>67</v>
       </c>
       <c r="R7" s="19" t="s">
@@ -1498,7 +1501,7 @@
       <c r="V7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="W7" s="21" t="s">
+      <c r="W7" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X7" s="19" t="s">
@@ -1510,7 +1513,7 @@
       <c r="Z7" s="10">
         <v>9.2200002670288086</v>
       </c>
-      <c r="AA7" s="20" t="s">
+      <c r="AA7" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB7" s="10">
@@ -1531,7 +1534,7 @@
       <c r="AG7" s="10">
         <v>9.3999996185302734</v>
       </c>
-      <c r="AH7" s="20" t="s">
+      <c r="AH7" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI7" s="10">
@@ -1568,13 +1571,13 @@
       <c r="N8" s="19"/>
       <c r="O8" s="19"/>
       <c r="P8" s="19"/>
-      <c r="Q8" s="21"/>
+      <c r="Q8" s="22"/>
       <c r="R8" s="19"/>
       <c r="S8" s="19"/>
       <c r="T8" s="19"/>
       <c r="U8" s="19"/>
       <c r="V8" s="19"/>
-      <c r="W8" s="21"/>
+      <c r="W8" s="22"/>
       <c r="X8" s="19"/>
       <c r="Y8" s="10">
         <v>20</v>
@@ -1582,7 +1585,7 @@
       <c r="Z8" s="10">
         <v>20.100000381469727</v>
       </c>
-      <c r="AA8" s="20"/>
+      <c r="AA8" s="23"/>
       <c r="AB8" s="10">
         <v>20.340000152587891</v>
       </c>
@@ -1601,7 +1604,7 @@
       <c r="AG8" s="10">
         <v>20</v>
       </c>
-      <c r="AH8" s="20"/>
+      <c r="AH8" s="23"/>
       <c r="AI8" s="10">
         <v>20.219999313354492</v>
       </c>
@@ -1693,7 +1696,7 @@
       <c r="L10" s="10">
         <v>10.039999999999999</v>
       </c>
-      <c r="M10" s="20" t="s">
+      <c r="M10" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N10" s="10">
@@ -1705,10 +1708,10 @@
       <c r="P10" s="10">
         <v>9.5699996948242188</v>
       </c>
-      <c r="Q10" s="21" t="s">
+      <c r="Q10" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R10" s="20" t="s">
+      <c r="R10" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S10" s="10">
@@ -1723,7 +1726,7 @@
       <c r="V10" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="W10" s="21" t="s">
+      <c r="W10" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X10" s="10">
@@ -1735,7 +1738,7 @@
       <c r="Z10" s="10">
         <v>10</v>
       </c>
-      <c r="AA10" s="20" t="s">
+      <c r="AA10" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB10" s="10">
@@ -1756,7 +1759,7 @@
       <c r="AG10" s="10">
         <v>10</v>
       </c>
-      <c r="AH10" s="20" t="s">
+      <c r="AH10" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI10" s="10">
@@ -1797,7 +1800,7 @@
       <c r="L11" s="10">
         <v>18.350000000000001</v>
       </c>
-      <c r="M11" s="20"/>
+      <c r="M11" s="23"/>
       <c r="N11" s="10">
         <v>18.489999771118164</v>
       </c>
@@ -1807,8 +1810,8 @@
       <c r="P11" s="10">
         <v>18.360000610351563</v>
       </c>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="20"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="23"/>
       <c r="S11" s="10">
         <v>18.3</v>
       </c>
@@ -1819,7 +1822,7 @@
         <v>18.3</v>
       </c>
       <c r="V11" s="19"/>
-      <c r="W11" s="21"/>
+      <c r="W11" s="22"/>
       <c r="X11" s="10">
         <v>18.379999160766602</v>
       </c>
@@ -1829,7 +1832,7 @@
       <c r="Z11" s="10">
         <v>19.059999465942383</v>
       </c>
-      <c r="AA11" s="20"/>
+      <c r="AA11" s="23"/>
       <c r="AB11" s="10">
         <v>19.420000076293945</v>
       </c>
@@ -1848,7 +1851,7 @@
       <c r="AG11" s="10">
         <v>18.350000381469727</v>
       </c>
-      <c r="AH11" s="20"/>
+      <c r="AH11" s="23"/>
       <c r="AI11" s="10">
         <v>18.5</v>
       </c>
@@ -1900,7 +1903,7 @@
       <c r="L13" s="10">
         <v>9.4499998092651367</v>
       </c>
-      <c r="M13" s="20" t="s">
+      <c r="M13" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N13" s="10">
@@ -1912,10 +1915,10 @@
       <c r="P13" s="10">
         <v>9.5500001907348633</v>
       </c>
-      <c r="Q13" s="21" t="s">
+      <c r="Q13" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R13" s="20" t="s">
+      <c r="R13" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S13" s="10">
@@ -1930,7 +1933,7 @@
       <c r="V13" s="10">
         <v>10</v>
       </c>
-      <c r="W13" s="21" t="s">
+      <c r="W13" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X13" s="10">
@@ -1942,7 +1945,7 @@
       <c r="Z13" s="10">
         <v>10.149999618530273</v>
       </c>
-      <c r="AA13" s="20" t="s">
+      <c r="AA13" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB13" s="10">
@@ -1963,7 +1966,7 @@
       <c r="AG13" s="10">
         <v>10</v>
       </c>
-      <c r="AH13" s="20" t="s">
+      <c r="AH13" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI13" s="19" t="s">
@@ -2000,7 +2003,7 @@
       <c r="L14" s="10">
         <v>18.319999694824219</v>
       </c>
-      <c r="M14" s="20"/>
+      <c r="M14" s="23"/>
       <c r="N14" s="10">
         <v>18.34</v>
       </c>
@@ -2010,8 +2013,8 @@
       <c r="P14" s="10">
         <v>18.3</v>
       </c>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="20"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="23"/>
       <c r="S14" s="10">
         <v>18.3</v>
       </c>
@@ -2024,7 +2027,7 @@
       <c r="V14" s="10">
         <v>18.3</v>
       </c>
-      <c r="W14" s="21"/>
+      <c r="W14" s="22"/>
       <c r="X14" s="10">
         <v>18.430000305175781</v>
       </c>
@@ -2034,7 +2037,7 @@
       <c r="Z14" s="10">
         <v>18.350000381469727</v>
       </c>
-      <c r="AA14" s="20"/>
+      <c r="AA14" s="23"/>
       <c r="AB14" s="10">
         <v>19.389999389648438</v>
       </c>
@@ -2053,7 +2056,7 @@
       <c r="AG14" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="AH14" s="20"/>
+      <c r="AH14" s="23"/>
       <c r="AI14" s="19"/>
       <c r="AJ14" s="10">
         <v>18.329999923706055</v>
@@ -2111,16 +2114,16 @@
       <c r="L16" s="10">
         <v>9.5799999237060547</v>
       </c>
-      <c r="M16" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="N16" s="23" t="s">
+      <c r="M16" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="O16" s="23" t="s">
+      <c r="O16" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="P16" s="23" t="s">
+      <c r="P16" s="21" t="s">
         <v>2</v>
       </c>
       <c r="Q16" s="19" t="s">
@@ -2141,7 +2144,7 @@
       <c r="V16" s="10">
         <v>10</v>
       </c>
-      <c r="W16" s="21" t="s">
+      <c r="W16" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X16" s="10">
@@ -2153,7 +2156,7 @@
       <c r="Z16" s="10">
         <v>9.5600004196166992</v>
       </c>
-      <c r="AA16" s="20" t="s">
+      <c r="AA16" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB16" s="10">
@@ -2174,7 +2177,7 @@
       <c r="AG16" s="10">
         <v>10</v>
       </c>
-      <c r="AH16" s="20" t="s">
+      <c r="AH16" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI16" s="10">
@@ -2215,10 +2218,10 @@
       <c r="L17" s="10">
         <v>18.3</v>
       </c>
-      <c r="M17" s="20"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
       <c r="Q17" s="19"/>
       <c r="R17" s="19"/>
       <c r="S17" s="19"/>
@@ -2229,7 +2232,7 @@
       <c r="V17" s="10">
         <v>18.3</v>
       </c>
-      <c r="W17" s="21"/>
+      <c r="W17" s="22"/>
       <c r="X17" s="10">
         <v>18.350000381469727</v>
       </c>
@@ -2239,7 +2242,7 @@
       <c r="Z17" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="AA17" s="20"/>
+      <c r="AA17" s="23"/>
       <c r="AB17" s="10">
         <v>19.360000610351563</v>
       </c>
@@ -2258,7 +2261,7 @@
       <c r="AG17" s="10">
         <v>18.3</v>
       </c>
-      <c r="AH17" s="20"/>
+      <c r="AH17" s="23"/>
       <c r="AI17" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -2309,7 +2312,7 @@
       <c r="I19" s="18">
         <v>9.5900001525878906</v>
       </c>
-      <c r="J19" s="22" t="s">
+      <c r="J19" s="20" t="s">
         <v>69</v>
       </c>
       <c r="K19" s="10">
@@ -2318,7 +2321,7 @@
       <c r="L19" s="10">
         <v>9.5799999237060547</v>
       </c>
-      <c r="M19" s="20" t="s">
+      <c r="M19" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N19" s="10">
@@ -2327,28 +2330,28 @@
       <c r="O19" s="10">
         <v>9.4700002670288086</v>
       </c>
-      <c r="P19" s="22" t="s">
+      <c r="P19" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="Q19" s="21" t="s">
+      <c r="Q19" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R19" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="S19" s="22" t="s">
+      <c r="R19" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="S19" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="T19" s="22" t="s">
+      <c r="T19" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="U19" s="22" t="s">
+      <c r="U19" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="V19" s="22" t="s">
+      <c r="V19" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="W19" s="21" t="s">
+      <c r="W19" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X19" s="10">
@@ -2360,7 +2363,7 @@
       <c r="Z19" s="10">
         <v>9.5299997329711914</v>
       </c>
-      <c r="AA19" s="20" t="s">
+      <c r="AA19" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB19" s="10">
@@ -2372,7 +2375,7 @@
       <c r="AD19" s="10">
         <v>9.5600004196166992</v>
       </c>
-      <c r="AE19" s="23" t="s">
+      <c r="AE19" s="21" t="s">
         <v>2</v>
       </c>
       <c r="AF19" s="10">
@@ -2381,7 +2384,7 @@
       <c r="AG19" s="10">
         <v>10</v>
       </c>
-      <c r="AH19" s="20" t="s">
+      <c r="AH19" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI19" s="10">
@@ -2397,7 +2400,7 @@
         <v>9.5500000000000007</v>
       </c>
       <c r="AM19" s="10">
-        <v>0</v>
+        <v>9.48</v>
       </c>
     </row>
     <row r="20" spans="1:39">
@@ -2413,28 +2416,28 @@
       <c r="I20" s="18">
         <v>18.329999923706055</v>
       </c>
-      <c r="J20" s="22"/>
+      <c r="J20" s="20"/>
       <c r="K20" s="10">
         <v>18.350000381469727</v>
       </c>
       <c r="L20" s="10">
         <v>18.3</v>
       </c>
-      <c r="M20" s="20"/>
+      <c r="M20" s="23"/>
       <c r="N20" s="10">
         <v>18.319999694824219</v>
       </c>
       <c r="O20" s="10">
         <v>18.340000152587891</v>
       </c>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="22"/>
-      <c r="U20" s="22"/>
-      <c r="V20" s="22"/>
-      <c r="W20" s="21"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="20"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="22"/>
       <c r="X20" s="10">
         <v>18.329999923706055</v>
       </c>
@@ -2444,7 +2447,7 @@
       <c r="Z20" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="AA20" s="20"/>
+      <c r="AA20" s="23"/>
       <c r="AB20" s="10">
         <v>19.360000610351563</v>
       </c>
@@ -2454,14 +2457,14 @@
       <c r="AD20" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="AE20" s="23"/>
+      <c r="AE20" s="21"/>
       <c r="AF20" s="10">
         <v>18.3</v>
       </c>
       <c r="AG20" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="AH20" s="20"/>
+      <c r="AH20" s="23"/>
       <c r="AI20" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -2472,10 +2475,10 @@
         <v>18.3</v>
       </c>
       <c r="AL20" s="10">
-        <v>0</v>
+        <v>18.309999999999999</v>
       </c>
       <c r="AM20" s="10">
-        <v>0</v>
+        <v>18.32</v>
       </c>
     </row>
     <row r="21" spans="1:39">
@@ -2521,7 +2524,7 @@
       <c r="L22" s="10">
         <v>10.06</v>
       </c>
-      <c r="M22" s="20" t="s">
+      <c r="M22" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N22" s="10">
@@ -2533,10 +2536,10 @@
       <c r="P22" s="10">
         <v>9.4600000381469727</v>
       </c>
-      <c r="Q22" s="21" t="s">
+      <c r="Q22" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R22" s="20" t="s">
+      <c r="R22" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S22" s="10">
@@ -2551,7 +2554,7 @@
       <c r="V22" s="10">
         <v>9.3500003814697266</v>
       </c>
-      <c r="W22" s="21" t="s">
+      <c r="W22" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X22" s="19" t="s">
@@ -2563,7 +2566,7 @@
       <c r="Z22" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AA22" s="20" t="s">
+      <c r="AA22" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB22" s="19" t="s">
@@ -2584,7 +2587,7 @@
       <c r="AG22" s="10">
         <v>10</v>
       </c>
-      <c r="AH22" s="20" t="s">
+      <c r="AH22" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI22" s="10">
@@ -2622,7 +2625,7 @@
       <c r="L23" s="10">
         <v>18.399999999999999</v>
       </c>
-      <c r="M23" s="20"/>
+      <c r="M23" s="23"/>
       <c r="N23" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -2632,8 +2635,8 @@
       <c r="P23" s="10">
         <v>18.360000610351563</v>
       </c>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="20"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="23"/>
       <c r="S23" s="10">
         <v>18.32</v>
       </c>
@@ -2646,11 +2649,11 @@
       <c r="V23" s="10">
         <v>13.520000457763672</v>
       </c>
-      <c r="W23" s="21"/>
+      <c r="W23" s="22"/>
       <c r="X23" s="19"/>
       <c r="Y23" s="19"/>
       <c r="Z23" s="19"/>
-      <c r="AA23" s="20"/>
+      <c r="AA23" s="23"/>
       <c r="AB23" s="19"/>
       <c r="AC23" s="19"/>
       <c r="AD23" s="19"/>
@@ -2663,7 +2666,7 @@
       <c r="AG23" s="10">
         <v>18.3</v>
       </c>
-      <c r="AH23" s="20"/>
+      <c r="AH23" s="23"/>
       <c r="AI23" s="10">
         <v>18.329999923706055</v>
       </c>
@@ -2731,7 +2734,7 @@
       <c r="L25" s="10">
         <v>10.210000000000001</v>
       </c>
-      <c r="M25" s="20" t="s">
+      <c r="M25" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N25" s="10">
@@ -2743,10 +2746,10 @@
       <c r="P25" s="10">
         <v>9.4600000381469727</v>
       </c>
-      <c r="Q25" s="21" t="s">
+      <c r="Q25" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R25" s="20" t="s">
+      <c r="R25" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S25" s="10">
@@ -2761,7 +2764,7 @@
       <c r="V25" s="10">
         <v>9.3500003814697266</v>
       </c>
-      <c r="W25" s="21" t="s">
+      <c r="W25" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X25" s="10">
@@ -2773,7 +2776,7 @@
       <c r="Z25" s="10">
         <v>0</v>
       </c>
-      <c r="AA25" s="20" t="s">
+      <c r="AA25" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB25" s="10">
@@ -2794,7 +2797,7 @@
       <c r="AG25" s="10">
         <v>10.27</v>
       </c>
-      <c r="AH25" s="20" t="s">
+      <c r="AH25" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI25" s="10">
@@ -2834,7 +2837,7 @@
       <c r="L26" s="10">
         <v>18.5</v>
       </c>
-      <c r="M26" s="20"/>
+      <c r="M26" s="23"/>
       <c r="N26" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -2844,8 +2847,8 @@
       <c r="P26" s="10">
         <v>18.360000610351563</v>
       </c>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="20"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="23"/>
       <c r="S26" s="10">
         <v>0</v>
       </c>
@@ -2858,7 +2861,7 @@
       <c r="V26" s="10">
         <v>13.520000457763672</v>
       </c>
-      <c r="W26" s="21"/>
+      <c r="W26" s="22"/>
       <c r="X26" s="10">
         <v>0</v>
       </c>
@@ -2868,7 +2871,7 @@
       <c r="Z26" s="10">
         <v>0</v>
       </c>
-      <c r="AA26" s="20"/>
+      <c r="AA26" s="23"/>
       <c r="AB26" s="10">
         <v>0</v>
       </c>
@@ -2887,7 +2890,7 @@
       <c r="AG26" s="10">
         <v>18.329999999999998</v>
       </c>
-      <c r="AH26" s="20"/>
+      <c r="AH26" s="23"/>
       <c r="AI26" s="10">
         <v>18.329999923706055</v>
       </c>
@@ -2946,7 +2949,7 @@
       <c r="L28" s="10">
         <v>9.5699996948242188</v>
       </c>
-      <c r="M28" s="20" t="s">
+      <c r="M28" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N28" s="10">
@@ -2958,10 +2961,10 @@
       <c r="P28" s="10">
         <v>9.5500001907348633</v>
       </c>
-      <c r="Q28" s="21" t="s">
+      <c r="Q28" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R28" s="20" t="s">
+      <c r="R28" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S28" s="10">
@@ -2976,7 +2979,7 @@
       <c r="V28" s="10">
         <v>10</v>
       </c>
-      <c r="W28" s="21" t="s">
+      <c r="W28" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X28" s="10">
@@ -2988,7 +2991,7 @@
       <c r="Z28" s="10">
         <v>9.5799999237060547</v>
       </c>
-      <c r="AA28" s="20" t="s">
+      <c r="AA28" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB28" s="10">
@@ -3009,7 +3012,7 @@
       <c r="AG28" s="10">
         <v>10</v>
       </c>
-      <c r="AH28" s="20" t="s">
+      <c r="AH28" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI28" s="10">
@@ -3049,7 +3052,7 @@
       <c r="L29" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="M29" s="20"/>
+      <c r="M29" s="23"/>
       <c r="N29" s="10">
         <v>18.340000152587891</v>
       </c>
@@ -3059,8 +3062,8 @@
       <c r="P29" s="10">
         <v>18.3</v>
       </c>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="20"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="23"/>
       <c r="S29" s="10">
         <v>18.3</v>
       </c>
@@ -3073,7 +3076,7 @@
       <c r="V29" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="W29" s="21"/>
+      <c r="W29" s="22"/>
       <c r="X29" s="10">
         <v>18.329999923706055</v>
       </c>
@@ -3083,7 +3086,7 @@
       <c r="Z29" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="AA29" s="20"/>
+      <c r="AA29" s="23"/>
       <c r="AB29" s="10">
         <v>19.370000839233398</v>
       </c>
@@ -3098,7 +3101,7 @@
       <c r="AG29" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="AH29" s="20"/>
+      <c r="AH29" s="23"/>
       <c r="AI29" s="10">
         <v>18.3</v>
       </c>
@@ -3157,7 +3160,7 @@
       <c r="L31" s="10">
         <v>9.4499998092651367</v>
       </c>
-      <c r="M31" s="20" t="s">
+      <c r="M31" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N31" s="10">
@@ -3169,10 +3172,10 @@
       <c r="P31" s="10">
         <v>9.5299997329711914</v>
       </c>
-      <c r="Q31" s="21" t="s">
+      <c r="Q31" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R31" s="20" t="s">
+      <c r="R31" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S31" s="10">
@@ -3187,7 +3190,7 @@
       <c r="V31" s="10">
         <v>10</v>
       </c>
-      <c r="W31" s="21" t="s">
+      <c r="W31" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X31" s="10">
@@ -3199,7 +3202,7 @@
       <c r="Z31" s="10">
         <v>9.5100002288818359</v>
       </c>
-      <c r="AA31" s="20" t="s">
+      <c r="AA31" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB31" s="10">
@@ -3220,7 +3223,7 @@
       <c r="AG31" s="10">
         <v>10</v>
       </c>
-      <c r="AH31" s="20" t="s">
+      <c r="AH31" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI31" s="10">
@@ -3260,7 +3263,7 @@
       <c r="L32" s="10">
         <v>18.319999694824219</v>
       </c>
-      <c r="M32" s="20"/>
+      <c r="M32" s="23"/>
       <c r="N32" s="10">
         <v>18.319999694824219</v>
       </c>
@@ -3270,8 +3273,8 @@
       <c r="P32" s="10">
         <v>18.3</v>
       </c>
-      <c r="Q32" s="21"/>
-      <c r="R32" s="20"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="23"/>
       <c r="S32" s="10">
         <v>18.3</v>
       </c>
@@ -3284,7 +3287,7 @@
       <c r="V32" s="10">
         <v>18.319999694824219</v>
       </c>
-      <c r="W32" s="21"/>
+      <c r="W32" s="22"/>
       <c r="X32" s="10">
         <v>18.329999923706055</v>
       </c>
@@ -3294,7 +3297,7 @@
       <c r="Z32" s="10">
         <v>18.350000381469727</v>
       </c>
-      <c r="AA32" s="20"/>
+      <c r="AA32" s="23"/>
       <c r="AB32" s="10">
         <v>19.360000610351563</v>
       </c>
@@ -3313,7 +3316,7 @@
       <c r="AG32" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="AH32" s="20"/>
+      <c r="AH32" s="23"/>
       <c r="AI32" s="10">
         <v>18.329999923706055</v>
       </c>
@@ -3372,7 +3375,7 @@
       <c r="L34" s="10">
         <v>9.4499998092651367</v>
       </c>
-      <c r="M34" s="20" t="s">
+      <c r="M34" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N34" s="10">
@@ -3384,10 +3387,10 @@
       <c r="P34" s="10">
         <v>9.4700002670288086</v>
       </c>
-      <c r="Q34" s="21" t="s">
+      <c r="Q34" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R34" s="20" t="s">
+      <c r="R34" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S34" s="10">
@@ -3402,7 +3405,7 @@
       <c r="V34" s="10">
         <v>9.369999885559082</v>
       </c>
-      <c r="W34" s="21" t="s">
+      <c r="W34" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X34" s="10">
@@ -3414,7 +3417,7 @@
       <c r="Z34" s="10">
         <v>9.3999996185302734</v>
       </c>
-      <c r="AA34" s="20" t="s">
+      <c r="AA34" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB34" s="10">
@@ -3435,7 +3438,7 @@
       <c r="AG34" s="10">
         <v>9.3999996185302734</v>
       </c>
-      <c r="AH34" s="20" t="s">
+      <c r="AH34" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI34" s="10">
@@ -3473,7 +3476,7 @@
       <c r="L35" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="M35" s="20"/>
+      <c r="M35" s="23"/>
       <c r="N35" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -3483,8 +3486,8 @@
       <c r="P35" s="10">
         <v>18.360000610351563</v>
       </c>
-      <c r="Q35" s="21"/>
-      <c r="R35" s="20"/>
+      <c r="Q35" s="22"/>
+      <c r="R35" s="23"/>
       <c r="S35" s="10">
         <v>18.3</v>
       </c>
@@ -3497,7 +3500,7 @@
       <c r="V35" s="10">
         <v>18.3</v>
       </c>
-      <c r="W35" s="21"/>
+      <c r="W35" s="22"/>
       <c r="X35" s="10">
         <v>18.319999694824219</v>
       </c>
@@ -3507,7 +3510,7 @@
       <c r="Z35" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="AA35" s="20"/>
+      <c r="AA35" s="23"/>
       <c r="AB35" s="10">
         <v>19.379999160766602</v>
       </c>
@@ -3526,7 +3529,7 @@
       <c r="AG35" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="AH35" s="20"/>
+      <c r="AH35" s="23"/>
       <c r="AI35" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -3583,7 +3586,7 @@
       <c r="L37" s="10">
         <v>9.1400003433227539</v>
       </c>
-      <c r="M37" s="20" t="s">
+      <c r="M37" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N37" s="10">
@@ -3595,10 +3598,10 @@
       <c r="P37" s="10">
         <v>8.5900001525878906</v>
       </c>
-      <c r="Q37" s="21" t="s">
+      <c r="Q37" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R37" s="20" t="s">
+      <c r="R37" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S37" s="10">
@@ -3613,7 +3616,7 @@
       <c r="V37" s="10">
         <v>8.5699996948242188</v>
       </c>
-      <c r="W37" s="21" t="s">
+      <c r="W37" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X37" s="10">
@@ -3625,7 +3628,7 @@
       <c r="Z37" s="10">
         <v>9.25</v>
       </c>
-      <c r="AA37" s="20" t="s">
+      <c r="AA37" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB37" s="10">
@@ -3646,7 +3649,7 @@
       <c r="AG37" s="10">
         <v>9.3999996185302734</v>
       </c>
-      <c r="AH37" s="20" t="s">
+      <c r="AH37" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI37" s="10">
@@ -3686,7 +3689,7 @@
       <c r="L38" s="10">
         <v>19.350000381469727</v>
       </c>
-      <c r="M38" s="20"/>
+      <c r="M38" s="23"/>
       <c r="N38" s="10">
         <v>19.350000381469727</v>
       </c>
@@ -3696,8 +3699,8 @@
       <c r="P38" s="10">
         <v>19.219999313354492</v>
       </c>
-      <c r="Q38" s="21"/>
-      <c r="R38" s="20"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="23"/>
       <c r="S38" s="10">
         <v>19.420000076293945</v>
       </c>
@@ -3710,7 +3713,7 @@
       <c r="V38" s="10">
         <v>19</v>
       </c>
-      <c r="W38" s="21"/>
+      <c r="W38" s="22"/>
       <c r="X38" s="10">
         <v>19.299999237060547</v>
       </c>
@@ -3720,7 +3723,7 @@
       <c r="Z38" s="10">
         <v>19.559999465942383</v>
       </c>
-      <c r="AA38" s="20"/>
+      <c r="AA38" s="23"/>
       <c r="AB38" s="10">
         <v>20.010000228881836</v>
       </c>
@@ -3739,7 +3742,7 @@
       <c r="AG38" s="10">
         <v>19.530000686645508</v>
       </c>
-      <c r="AH38" s="20"/>
+      <c r="AH38" s="23"/>
       <c r="AI38" s="10">
         <v>20</v>
       </c>
@@ -3807,7 +3810,7 @@
       <c r="L40" s="10">
         <v>9.4499998092651367</v>
       </c>
-      <c r="M40" s="20" t="s">
+      <c r="M40" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N40" s="10">
@@ -3819,10 +3822,10 @@
       <c r="P40" s="10">
         <v>9.4700002670288086</v>
       </c>
-      <c r="Q40" s="21" t="s">
+      <c r="Q40" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R40" s="20" t="s">
+      <c r="R40" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S40" s="10">
@@ -3837,7 +3840,7 @@
       <c r="V40" s="10">
         <v>9.5699996948242188</v>
       </c>
-      <c r="W40" s="21" t="s">
+      <c r="W40" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X40" s="10">
@@ -3849,7 +3852,7 @@
       <c r="Z40" s="10">
         <v>9.5799999237060547</v>
       </c>
-      <c r="AA40" s="20" t="s">
+      <c r="AA40" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB40" s="10">
@@ -3870,7 +3873,7 @@
       <c r="AG40" s="10">
         <v>10</v>
       </c>
-      <c r="AH40" s="20" t="s">
+      <c r="AH40" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI40" s="10">
@@ -3910,7 +3913,7 @@
       <c r="L41" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="M41" s="20"/>
+      <c r="M41" s="23"/>
       <c r="N41" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -3920,8 +3923,8 @@
       <c r="P41" s="10">
         <v>18.190000534057617</v>
       </c>
-      <c r="Q41" s="21"/>
-      <c r="R41" s="20"/>
+      <c r="Q41" s="22"/>
+      <c r="R41" s="23"/>
       <c r="S41" s="10">
         <v>18.3</v>
       </c>
@@ -3934,7 +3937,7 @@
       <c r="V41" s="10">
         <v>18.3</v>
       </c>
-      <c r="W41" s="21"/>
+      <c r="W41" s="22"/>
       <c r="X41" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -3942,7 +3945,7 @@
       <c r="Z41" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="AA41" s="20"/>
+      <c r="AA41" s="23"/>
       <c r="AB41" s="10">
         <v>19.360000610351563</v>
       </c>
@@ -3961,7 +3964,7 @@
       <c r="AG41" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="AH41" s="20"/>
+      <c r="AH41" s="23"/>
       <c r="AI41" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -4018,7 +4021,7 @@
       <c r="L43" s="10">
         <v>10.5</v>
       </c>
-      <c r="M43" s="20" t="s">
+      <c r="M43" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N43" s="10">
@@ -4030,10 +4033,10 @@
       <c r="P43" s="10">
         <v>9.5699996948242188</v>
       </c>
-      <c r="Q43" s="21" t="s">
+      <c r="Q43" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R43" s="20" t="s">
+      <c r="R43" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S43" s="10">
@@ -4048,7 +4051,7 @@
       <c r="V43" s="10">
         <v>10</v>
       </c>
-      <c r="W43" s="21" t="s">
+      <c r="W43" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X43" s="10">
@@ -4060,7 +4063,7 @@
       <c r="Z43" s="10">
         <v>9.5500001907348633</v>
       </c>
-      <c r="AA43" s="20" t="s">
+      <c r="AA43" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB43" s="10">
@@ -4081,7 +4084,7 @@
       <c r="AG43" s="10">
         <v>10.090000152587891</v>
       </c>
-      <c r="AH43" s="20" t="s">
+      <c r="AH43" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI43" s="10">
@@ -4119,7 +4122,7 @@
       <c r="L44" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="M44" s="20"/>
+      <c r="M44" s="23"/>
       <c r="N44" s="10">
         <v>18.319999694824219</v>
       </c>
@@ -4129,8 +4132,8 @@
       <c r="P44" s="10">
         <v>18.340000152587891</v>
       </c>
-      <c r="Q44" s="21"/>
-      <c r="R44" s="20"/>
+      <c r="Q44" s="22"/>
+      <c r="R44" s="23"/>
       <c r="S44" s="10">
         <v>18.329999923706055</v>
       </c>
@@ -4141,7 +4144,7 @@
       <c r="V44" s="10">
         <v>18.3</v>
       </c>
-      <c r="W44" s="21"/>
+      <c r="W44" s="22"/>
       <c r="X44" s="10">
         <v>18.340000152587891</v>
       </c>
@@ -4151,7 +4154,7 @@
       <c r="Z44" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="AA44" s="20"/>
+      <c r="AA44" s="23"/>
       <c r="AB44" s="10">
         <v>19.360000610351563</v>
       </c>
@@ -4170,7 +4173,7 @@
       <c r="AG44" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="AH44" s="20"/>
+      <c r="AH44" s="23"/>
       <c r="AI44" s="10">
         <v>18.3</v>
       </c>
@@ -4225,7 +4228,7 @@
       <c r="L46" s="10">
         <v>9.4499998092651367</v>
       </c>
-      <c r="M46" s="20" t="s">
+      <c r="M46" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N46" s="10">
@@ -4255,7 +4258,7 @@
       <c r="V46" s="10">
         <v>9.130000114440918</v>
       </c>
-      <c r="W46" s="21" t="s">
+      <c r="W46" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X46" s="10">
@@ -4267,7 +4270,7 @@
       <c r="Z46" s="10">
         <v>9.2200002670288086</v>
       </c>
-      <c r="AA46" s="20" t="s">
+      <c r="AA46" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB46" s="10">
@@ -4288,7 +4291,7 @@
       <c r="AG46" s="10">
         <v>9.3999996185302734</v>
       </c>
-      <c r="AH46" s="20" t="s">
+      <c r="AH46" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI46" s="10">
@@ -4325,7 +4328,7 @@
       <c r="L47" s="10">
         <v>18.319999694824219</v>
       </c>
-      <c r="M47" s="20"/>
+      <c r="M47" s="23"/>
       <c r="N47" s="10">
         <v>18.3</v>
       </c>
@@ -4341,7 +4344,7 @@
       <c r="V47" s="10">
         <v>18.3</v>
       </c>
-      <c r="W47" s="21"/>
+      <c r="W47" s="22"/>
       <c r="X47" s="10">
         <v>18.340000152587891</v>
       </c>
@@ -4351,7 +4354,7 @@
       <c r="Z47" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="AA47" s="20"/>
+      <c r="AA47" s="23"/>
       <c r="AB47" s="10">
         <v>19.379999160766602</v>
       </c>
@@ -4370,7 +4373,7 @@
       <c r="AG47" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="AH47" s="20"/>
+      <c r="AH47" s="23"/>
       <c r="AI47" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -4418,7 +4421,7 @@
       <c r="L49" s="10">
         <v>10.43</v>
       </c>
-      <c r="M49" s="20" t="s">
+      <c r="M49" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N49" s="10">
@@ -4430,10 +4433,10 @@
       <c r="P49" s="10">
         <v>9.5399999618530273</v>
       </c>
-      <c r="Q49" s="21" t="s">
+      <c r="Q49" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R49" s="20" t="s">
+      <c r="R49" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S49" s="10">
@@ -4481,7 +4484,7 @@
       <c r="AG49" s="10">
         <v>10</v>
       </c>
-      <c r="AH49" s="20" t="s">
+      <c r="AH49" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI49" s="10">
@@ -4518,7 +4521,7 @@
       <c r="L50" s="10">
         <v>18.3</v>
       </c>
-      <c r="M50" s="20"/>
+      <c r="M50" s="23"/>
       <c r="N50" s="10">
         <v>18.329999923706055</v>
       </c>
@@ -4528,8 +4531,8 @@
       <c r="P50" s="10">
         <v>17.559999465942383</v>
       </c>
-      <c r="Q50" s="21"/>
-      <c r="R50" s="20"/>
+      <c r="Q50" s="22"/>
+      <c r="R50" s="23"/>
       <c r="S50" s="10">
         <v>18.3</v>
       </c>
@@ -4559,7 +4562,7 @@
       <c r="AG50" s="10">
         <v>18.36</v>
       </c>
-      <c r="AH50" s="20"/>
+      <c r="AH50" s="23"/>
       <c r="AI50" s="10">
         <v>18.3</v>
       </c>
@@ -4589,7 +4592,7 @@
       </c>
       <c r="C52" s="15"/>
       <c r="D52" s="5" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="E52" s="12" t="s">
         <v>51</v>
@@ -4615,7 +4618,7 @@
       <c r="L52" s="10">
         <v>10.039999961853027</v>
       </c>
-      <c r="M52" s="20" t="s">
+      <c r="M52" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N52" s="19" t="s">
@@ -4627,10 +4630,10 @@
       <c r="P52" s="10">
         <v>9.5900001525878906</v>
       </c>
-      <c r="Q52" s="21" t="s">
+      <c r="Q52" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R52" s="20" t="s">
+      <c r="R52" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S52" s="10">
@@ -4645,7 +4648,7 @@
       <c r="V52" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="W52" s="21" t="s">
+      <c r="W52" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X52" s="10">
@@ -4657,7 +4660,7 @@
       <c r="Z52" s="10">
         <v>10.149999618530273</v>
       </c>
-      <c r="AA52" s="20" t="s">
+      <c r="AA52" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB52" s="10">
@@ -4678,7 +4681,7 @@
       <c r="AG52" s="10">
         <v>10</v>
       </c>
-      <c r="AH52" s="20" t="s">
+      <c r="AH52" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI52" s="10">
@@ -4715,14 +4718,14 @@
       <c r="L53" s="10">
         <v>18.340000152587891</v>
       </c>
-      <c r="M53" s="20"/>
+      <c r="M53" s="23"/>
       <c r="N53" s="19"/>
       <c r="O53" s="19"/>
       <c r="P53" s="10">
         <v>18.340000152587891</v>
       </c>
-      <c r="Q53" s="21"/>
-      <c r="R53" s="20"/>
+      <c r="Q53" s="22"/>
+      <c r="R53" s="23"/>
       <c r="S53" s="10">
         <v>18.329999923706055</v>
       </c>
@@ -4733,7 +4736,7 @@
         <v>18.329999923706055</v>
       </c>
       <c r="V53" s="19"/>
-      <c r="W53" s="21"/>
+      <c r="W53" s="22"/>
       <c r="X53" s="10">
         <v>18.319999694824219</v>
       </c>
@@ -4743,7 +4746,7 @@
       <c r="Z53" s="10">
         <v>18.370000839233398</v>
       </c>
-      <c r="AA53" s="20"/>
+      <c r="AA53" s="23"/>
       <c r="AB53" s="10">
         <v>18.32</v>
       </c>
@@ -4762,7 +4765,7 @@
       <c r="AG53" s="10">
         <v>0</v>
       </c>
-      <c r="AH53" s="20"/>
+      <c r="AH53" s="23"/>
       <c r="AI53" s="10">
         <v>18.350000381469727</v>
       </c>
@@ -4827,7 +4830,7 @@
       <c r="L55" s="10">
         <v>9.3299999237060547</v>
       </c>
-      <c r="M55" s="20" t="s">
+      <c r="M55" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N55" s="10">
@@ -4839,10 +4842,10 @@
       <c r="P55" s="10">
         <v>10</v>
       </c>
-      <c r="Q55" s="21" t="s">
+      <c r="Q55" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R55" s="20" t="s">
+      <c r="R55" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S55" s="10">
@@ -4857,7 +4860,7 @@
       <c r="V55" s="10">
         <v>9.5900001525878906</v>
       </c>
-      <c r="W55" s="21" t="s">
+      <c r="W55" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X55" s="10">
@@ -4869,7 +4872,7 @@
       <c r="Z55" s="10">
         <v>9.4099998474121094</v>
       </c>
-      <c r="AA55" s="20" t="s">
+      <c r="AA55" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB55" s="10">
@@ -4890,7 +4893,7 @@
       <c r="AG55" s="10">
         <v>10</v>
       </c>
-      <c r="AH55" s="20" t="s">
+      <c r="AH55" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI55" s="10">
@@ -4928,7 +4931,7 @@
       <c r="L56" s="10">
         <v>18.3</v>
       </c>
-      <c r="M56" s="20"/>
+      <c r="M56" s="23"/>
       <c r="N56" s="10">
         <v>18.319999694824219</v>
       </c>
@@ -4938,8 +4941,8 @@
       <c r="P56" s="10">
         <v>16</v>
       </c>
-      <c r="Q56" s="21"/>
-      <c r="R56" s="20"/>
+      <c r="Q56" s="22"/>
+      <c r="R56" s="23"/>
       <c r="S56" s="10">
         <v>18.319999694824219</v>
       </c>
@@ -4950,7 +4953,7 @@
       <c r="V56" s="10">
         <v>18.3</v>
       </c>
-      <c r="W56" s="21"/>
+      <c r="W56" s="22"/>
       <c r="X56" s="10">
         <v>18.319999694824219</v>
       </c>
@@ -4960,7 +4963,7 @@
       <c r="Z56" s="10">
         <v>18.319999694824219</v>
       </c>
-      <c r="AA56" s="20"/>
+      <c r="AA56" s="23"/>
       <c r="AB56" s="10">
         <v>19.389999389648438</v>
       </c>
@@ -4977,7 +4980,7 @@
       <c r="AG56" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="AH56" s="20"/>
+      <c r="AH56" s="23"/>
       <c r="AI56" s="10">
         <v>18.3</v>
       </c>
@@ -5034,7 +5037,7 @@
       <c r="L58" s="10">
         <v>9.3299999237060547</v>
       </c>
-      <c r="M58" s="20" t="s">
+      <c r="M58" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N58" s="10">
@@ -5046,10 +5049,10 @@
       <c r="P58" s="10">
         <v>9.4399995803833008</v>
       </c>
-      <c r="Q58" s="21" t="s">
+      <c r="Q58" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R58" s="20" t="s">
+      <c r="R58" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S58" s="10">
@@ -5064,7 +5067,7 @@
       <c r="V58" s="10">
         <v>9.59</v>
       </c>
-      <c r="W58" s="21" t="s">
+      <c r="W58" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X58" s="19" t="s">
@@ -5076,7 +5079,7 @@
       <c r="Z58" s="10">
         <v>9.4099998474121094</v>
       </c>
-      <c r="AA58" s="20" t="s">
+      <c r="AA58" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB58" s="10">
@@ -5097,7 +5100,7 @@
       <c r="AG58" s="10">
         <v>10</v>
       </c>
-      <c r="AH58" s="20" t="s">
+      <c r="AH58" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI58" s="10">
@@ -5134,7 +5137,7 @@
       <c r="L59" s="10">
         <v>18.3</v>
       </c>
-      <c r="M59" s="20"/>
+      <c r="M59" s="23"/>
       <c r="N59" s="10">
         <v>18.319999694824219</v>
       </c>
@@ -5144,8 +5147,8 @@
       <c r="P59" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="Q59" s="21"/>
-      <c r="R59" s="20"/>
+      <c r="Q59" s="22"/>
+      <c r="R59" s="23"/>
       <c r="S59" s="10">
         <v>18.3</v>
       </c>
@@ -5158,13 +5161,13 @@
       <c r="V59" s="10">
         <v>18.3</v>
       </c>
-      <c r="W59" s="21"/>
+      <c r="W59" s="22"/>
       <c r="X59" s="19"/>
       <c r="Y59" s="19"/>
       <c r="Z59" s="10">
         <v>18.319999694824219</v>
       </c>
-      <c r="AA59" s="20"/>
+      <c r="AA59" s="23"/>
       <c r="AB59" s="10">
         <v>19.389999389648438</v>
       </c>
@@ -5183,7 +5186,7 @@
       <c r="AG59" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="AH59" s="20"/>
+      <c r="AH59" s="23"/>
       <c r="AI59" s="10">
         <v>18.3</v>
       </c>
@@ -5235,7 +5238,7 @@
       <c r="L61" s="10">
         <v>10.060000419616699</v>
       </c>
-      <c r="M61" s="20" t="s">
+      <c r="M61" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N61" s="10">
@@ -5247,10 +5250,10 @@
       <c r="P61" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="Q61" s="21" t="s">
+      <c r="Q61" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R61" s="20" t="s">
+      <c r="R61" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S61" s="10">
@@ -5265,7 +5268,7 @@
       <c r="V61" s="10">
         <v>10</v>
       </c>
-      <c r="W61" s="21" t="s">
+      <c r="W61" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X61" s="10">
@@ -5277,7 +5280,7 @@
       <c r="Z61" s="10">
         <v>9.5600004196166992</v>
       </c>
-      <c r="AA61" s="20" t="s">
+      <c r="AA61" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB61" s="10">
@@ -5298,7 +5301,7 @@
       <c r="AG61" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AH61" s="20" t="s">
+      <c r="AH61" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI61" s="10">
@@ -5336,7 +5339,7 @@
       <c r="L62" s="10">
         <v>18.319999694824219</v>
       </c>
-      <c r="M62" s="20"/>
+      <c r="M62" s="23"/>
       <c r="N62" s="10">
         <v>18.329999923706055</v>
       </c>
@@ -5344,8 +5347,8 @@
         <v>18.309999465942383</v>
       </c>
       <c r="P62" s="19"/>
-      <c r="Q62" s="21"/>
-      <c r="R62" s="20"/>
+      <c r="Q62" s="22"/>
+      <c r="R62" s="23"/>
       <c r="S62" s="10">
         <v>18.3</v>
       </c>
@@ -5358,7 +5361,7 @@
       <c r="V62" s="10">
         <v>18.3</v>
       </c>
-      <c r="W62" s="21"/>
+      <c r="W62" s="22"/>
       <c r="X62" s="10">
         <v>18.319999694824219</v>
       </c>
@@ -5368,7 +5371,7 @@
       <c r="Z62" s="10">
         <v>18.3</v>
       </c>
-      <c r="AA62" s="20"/>
+      <c r="AA62" s="23"/>
       <c r="AB62" s="10">
         <v>19.379999160766602</v>
       </c>
@@ -5385,7 +5388,7 @@
         <v>18.3</v>
       </c>
       <c r="AG62" s="19"/>
-      <c r="AH62" s="20"/>
+      <c r="AH62" s="23"/>
       <c r="AI62" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -5437,7 +5440,7 @@
       <c r="L64" s="10">
         <v>9.5600004196166992</v>
       </c>
-      <c r="M64" s="20" t="s">
+      <c r="M64" s="23" t="s">
         <v>0</v>
       </c>
       <c r="N64" s="10">
@@ -5449,10 +5452,10 @@
       <c r="P64" s="10">
         <v>9.5200004577636719</v>
       </c>
-      <c r="Q64" s="21" t="s">
+      <c r="Q64" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="R64" s="20" t="s">
+      <c r="R64" s="23" t="s">
         <v>0</v>
       </c>
       <c r="S64" s="10">
@@ -5467,7 +5470,7 @@
       <c r="V64" s="10">
         <v>9.5600004196166992</v>
       </c>
-      <c r="W64" s="21" t="s">
+      <c r="W64" s="22" t="s">
         <v>67</v>
       </c>
       <c r="X64" s="10">
@@ -5479,7 +5482,7 @@
       <c r="Z64" s="10">
         <v>12.119999885559082</v>
       </c>
-      <c r="AA64" s="20" t="s">
+      <c r="AA64" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AB64" s="10">
@@ -5500,7 +5503,7 @@
       <c r="AG64" s="10">
         <v>10</v>
       </c>
-      <c r="AH64" s="20" t="s">
+      <c r="AH64" s="23" t="s">
         <v>0</v>
       </c>
       <c r="AI64" s="10">
@@ -5538,7 +5541,7 @@
       <c r="L65" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="M65" s="20"/>
+      <c r="M65" s="23"/>
       <c r="N65" s="10">
         <v>18.319999694824219</v>
       </c>
@@ -5548,8 +5551,8 @@
       <c r="P65" s="10">
         <v>18.309999465942383</v>
       </c>
-      <c r="Q65" s="21"/>
-      <c r="R65" s="20"/>
+      <c r="Q65" s="22"/>
+      <c r="R65" s="23"/>
       <c r="S65" s="10">
         <v>18.3</v>
       </c>
@@ -5562,7 +5565,7 @@
       <c r="V65" s="10">
         <v>18.3</v>
       </c>
-      <c r="W65" s="21"/>
+      <c r="W65" s="22"/>
       <c r="X65" s="10">
         <v>18.350000381469727</v>
       </c>
@@ -5570,7 +5573,7 @@
       <c r="Z65" s="10">
         <v>18.329999923706055</v>
       </c>
-      <c r="AA65" s="20"/>
+      <c r="AA65" s="23"/>
       <c r="AB65" s="10">
         <v>18.3</v>
       </c>
@@ -5589,7 +5592,7 @@
       <c r="AG65" s="10">
         <v>18.370000839233398</v>
       </c>
-      <c r="AH65" s="20"/>
+      <c r="AH65" s="23"/>
       <c r="AI65" s="10">
         <v>18.309999465942383</v>
       </c>
@@ -5607,28 +5610,28 @@
       </c>
     </row>
     <row r="75" spans="2:39">
-      <c r="B75" s="21" t="s">
+      <c r="B75" s="22" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="76" spans="2:39">
-      <c r="B76" s="21"/>
+      <c r="B76" s="22"/>
     </row>
     <row r="77" spans="2:39">
-      <c r="B77" s="22" t="s">
+      <c r="B77" s="20" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="78" spans="2:39">
-      <c r="B78" s="22"/>
+      <c r="B78" s="20"/>
     </row>
     <row r="79" spans="2:39">
-      <c r="B79" s="23" t="s">
+      <c r="B79" s="21" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="80" spans="2:39">
-      <c r="B80" s="23"/>
+      <c r="B80" s="21"/>
     </row>
     <row r="81" spans="2:2">
       <c r="B81" s="19" t="s">
@@ -5640,168 +5643,27 @@
     </row>
   </sheetData>
   <mergeCells count="206">
-    <mergeCell ref="AM46:AM47"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="AI13:AI14"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="AE19:AE20"/>
-    <mergeCell ref="W22:W23"/>
-    <mergeCell ref="W25:W26"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="AI4:AI5"/>
-    <mergeCell ref="AJ4:AJ5"/>
-    <mergeCell ref="AK4:AK5"/>
-    <mergeCell ref="AL4:AL5"/>
-    <mergeCell ref="AM4:AM5"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="X22:X23"/>
-    <mergeCell ref="Y22:Y23"/>
-    <mergeCell ref="Z22:Z23"/>
-    <mergeCell ref="AB22:AB23"/>
-    <mergeCell ref="AC22:AC23"/>
-    <mergeCell ref="AD22:AD23"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="S16:S17"/>
-    <mergeCell ref="T16:T17"/>
-    <mergeCell ref="V10:V11"/>
-    <mergeCell ref="AJ10:AJ11"/>
-    <mergeCell ref="AK10:AK11"/>
-    <mergeCell ref="AL10:AL11"/>
-    <mergeCell ref="AM10:AM11"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="AL34:AL35"/>
-    <mergeCell ref="Y40:Y41"/>
-    <mergeCell ref="AK40:AK41"/>
-    <mergeCell ref="P46:P47"/>
-    <mergeCell ref="S46:S47"/>
-    <mergeCell ref="T46:T47"/>
-    <mergeCell ref="U46:U47"/>
-    <mergeCell ref="AJ46:AJ47"/>
-    <mergeCell ref="U55:U56"/>
-    <mergeCell ref="AD55:AD56"/>
-    <mergeCell ref="W34:W35"/>
-    <mergeCell ref="R40:R41"/>
-    <mergeCell ref="AK46:AK47"/>
-    <mergeCell ref="AL46:AL47"/>
-    <mergeCell ref="V49:V50"/>
-    <mergeCell ref="X49:X50"/>
-    <mergeCell ref="Y49:Y50"/>
-    <mergeCell ref="Z49:Z50"/>
-    <mergeCell ref="AB49:AB50"/>
-    <mergeCell ref="AC49:AC50"/>
-    <mergeCell ref="Y64:Y65"/>
-    <mergeCell ref="U43:U44"/>
-    <mergeCell ref="AJ43:AJ44"/>
-    <mergeCell ref="AG61:AG62"/>
-    <mergeCell ref="X58:X59"/>
-    <mergeCell ref="Y58:Y59"/>
-    <mergeCell ref="W52:W53"/>
-    <mergeCell ref="T19:T20"/>
-    <mergeCell ref="AA4:AA5"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="R25:R26"/>
+    <mergeCell ref="R28:R29"/>
+    <mergeCell ref="R31:R32"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="R46:R47"/>
+    <mergeCell ref="R49:R50"/>
+    <mergeCell ref="R52:R53"/>
+    <mergeCell ref="R55:R56"/>
+    <mergeCell ref="R58:R59"/>
+    <mergeCell ref="R61:R62"/>
+    <mergeCell ref="M31:M32"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="P61:P62"/>
+    <mergeCell ref="R64:R65"/>
     <mergeCell ref="M55:M56"/>
-    <mergeCell ref="W55:W56"/>
-    <mergeCell ref="M58:M59"/>
-    <mergeCell ref="W58:W59"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="W4:W5"/>
-    <mergeCell ref="W10:W11"/>
-    <mergeCell ref="W13:W14"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="N52:N53"/>
-    <mergeCell ref="O52:O53"/>
-    <mergeCell ref="V52:V53"/>
-    <mergeCell ref="AH19:AH20"/>
-    <mergeCell ref="AH28:AH29"/>
-    <mergeCell ref="AH37:AH38"/>
-    <mergeCell ref="AH40:AH41"/>
-    <mergeCell ref="AH43:AH44"/>
-    <mergeCell ref="AH46:AH47"/>
-    <mergeCell ref="W46:W47"/>
-    <mergeCell ref="W49:W50"/>
-    <mergeCell ref="W37:W38"/>
-    <mergeCell ref="W40:W41"/>
-    <mergeCell ref="W43:W44"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="AH31:AH32"/>
-    <mergeCell ref="AH34:AH35"/>
-    <mergeCell ref="AD28:AD29"/>
-    <mergeCell ref="AE28:AE29"/>
-    <mergeCell ref="W28:W29"/>
-    <mergeCell ref="W31:W32"/>
-    <mergeCell ref="AH4:AH5"/>
-    <mergeCell ref="AA34:AA35"/>
-    <mergeCell ref="AA37:AA38"/>
-    <mergeCell ref="AA40:AA41"/>
-    <mergeCell ref="AA43:AA44"/>
-    <mergeCell ref="AA46:AA47"/>
-    <mergeCell ref="AA49:AA50"/>
-    <mergeCell ref="AA52:AA53"/>
-    <mergeCell ref="AA55:AA56"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AA10:AA11"/>
-    <mergeCell ref="AA13:AA14"/>
-    <mergeCell ref="AA16:AA17"/>
-    <mergeCell ref="AA19:AA20"/>
-    <mergeCell ref="AA22:AA23"/>
-    <mergeCell ref="AA25:AA26"/>
-    <mergeCell ref="AA28:AA29"/>
-    <mergeCell ref="AA31:AA32"/>
-    <mergeCell ref="AH7:AH8"/>
-    <mergeCell ref="AH10:AH11"/>
-    <mergeCell ref="AH13:AH14"/>
-    <mergeCell ref="AH16:AH17"/>
-    <mergeCell ref="AH22:AH23"/>
-    <mergeCell ref="AH25:AH26"/>
-    <mergeCell ref="AH61:AH62"/>
-    <mergeCell ref="R19:R20"/>
-    <mergeCell ref="S19:S20"/>
-    <mergeCell ref="AH49:AH50"/>
-    <mergeCell ref="AH52:AH53"/>
-    <mergeCell ref="AH55:AH56"/>
-    <mergeCell ref="AH58:AH59"/>
-    <mergeCell ref="AA61:AA62"/>
-    <mergeCell ref="M64:M65"/>
-    <mergeCell ref="AA64:AA65"/>
-    <mergeCell ref="AH64:AH65"/>
-    <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="Q52:Q53"/>
-    <mergeCell ref="Q55:Q56"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="R34:R35"/>
-    <mergeCell ref="R37:R38"/>
-    <mergeCell ref="M61:M62"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="M52:M53"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="M46:M47"/>
-    <mergeCell ref="M49:M50"/>
     <mergeCell ref="B77:B78"/>
     <mergeCell ref="B79:B80"/>
     <mergeCell ref="B81:B82"/>
@@ -5826,26 +5688,167 @@
     <mergeCell ref="Q43:Q44"/>
     <mergeCell ref="Q46:Q47"/>
     <mergeCell ref="R43:R44"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="R16:R17"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="R25:R26"/>
-    <mergeCell ref="R28:R29"/>
-    <mergeCell ref="R31:R32"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="R46:R47"/>
-    <mergeCell ref="R49:R50"/>
-    <mergeCell ref="R52:R53"/>
-    <mergeCell ref="R55:R56"/>
-    <mergeCell ref="R58:R59"/>
-    <mergeCell ref="R61:R62"/>
-    <mergeCell ref="M31:M32"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="M37:M38"/>
-    <mergeCell ref="P61:P62"/>
-    <mergeCell ref="R64:R65"/>
+    <mergeCell ref="M64:M65"/>
+    <mergeCell ref="AA64:AA65"/>
+    <mergeCell ref="AH64:AH65"/>
+    <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="Q52:Q53"/>
+    <mergeCell ref="Q55:Q56"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="R34:R35"/>
+    <mergeCell ref="R37:R38"/>
+    <mergeCell ref="M61:M62"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="M52:M53"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="M46:M47"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="AH19:AH20"/>
+    <mergeCell ref="AH28:AH29"/>
+    <mergeCell ref="AH16:AH17"/>
+    <mergeCell ref="AH22:AH23"/>
+    <mergeCell ref="AH25:AH26"/>
+    <mergeCell ref="S19:S20"/>
+    <mergeCell ref="AH49:AH50"/>
+    <mergeCell ref="AH52:AH53"/>
+    <mergeCell ref="AH55:AH56"/>
+    <mergeCell ref="AH58:AH59"/>
+    <mergeCell ref="AA61:AA62"/>
+    <mergeCell ref="AH31:AH32"/>
+    <mergeCell ref="AH34:AH35"/>
+    <mergeCell ref="AD28:AD29"/>
+    <mergeCell ref="AE28:AE29"/>
+    <mergeCell ref="W28:W29"/>
+    <mergeCell ref="W31:W32"/>
+    <mergeCell ref="T19:T20"/>
+    <mergeCell ref="AA4:AA5"/>
+    <mergeCell ref="AH37:AH38"/>
+    <mergeCell ref="W37:W38"/>
+    <mergeCell ref="AH4:AH5"/>
+    <mergeCell ref="AA34:AA35"/>
+    <mergeCell ref="AA37:AA38"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AA10:AA11"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="AA16:AA17"/>
+    <mergeCell ref="AA19:AA20"/>
+    <mergeCell ref="AA22:AA23"/>
+    <mergeCell ref="AA25:AA26"/>
+    <mergeCell ref="AA28:AA29"/>
+    <mergeCell ref="AA31:AA32"/>
+    <mergeCell ref="AH7:AH8"/>
+    <mergeCell ref="AH10:AH11"/>
+    <mergeCell ref="M58:M59"/>
+    <mergeCell ref="W58:W59"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="W4:W5"/>
+    <mergeCell ref="W10:W11"/>
+    <mergeCell ref="W13:W14"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="O52:O53"/>
+    <mergeCell ref="V52:V53"/>
+    <mergeCell ref="R19:R20"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W46:W47"/>
+    <mergeCell ref="W49:W50"/>
+    <mergeCell ref="AL46:AL47"/>
+    <mergeCell ref="V49:V50"/>
+    <mergeCell ref="X49:X50"/>
+    <mergeCell ref="Y49:Y50"/>
+    <mergeCell ref="Z49:Z50"/>
+    <mergeCell ref="AB49:AB50"/>
+    <mergeCell ref="AC49:AC50"/>
+    <mergeCell ref="Y64:Y65"/>
+    <mergeCell ref="U43:U44"/>
+    <mergeCell ref="AJ43:AJ44"/>
+    <mergeCell ref="AG61:AG62"/>
+    <mergeCell ref="X58:X59"/>
+    <mergeCell ref="Y58:Y59"/>
+    <mergeCell ref="W52:W53"/>
+    <mergeCell ref="AH61:AH62"/>
+    <mergeCell ref="W55:W56"/>
+    <mergeCell ref="AH43:AH44"/>
+    <mergeCell ref="AH46:AH47"/>
+    <mergeCell ref="W43:W44"/>
+    <mergeCell ref="AA43:AA44"/>
+    <mergeCell ref="AA46:AA47"/>
+    <mergeCell ref="AA49:AA50"/>
+    <mergeCell ref="AA52:AA53"/>
+    <mergeCell ref="AA55:AA56"/>
+    <mergeCell ref="AK40:AK41"/>
+    <mergeCell ref="P46:P47"/>
+    <mergeCell ref="S46:S47"/>
+    <mergeCell ref="T46:T47"/>
+    <mergeCell ref="U46:U47"/>
+    <mergeCell ref="AJ46:AJ47"/>
+    <mergeCell ref="U55:U56"/>
+    <mergeCell ref="AD55:AD56"/>
+    <mergeCell ref="W34:W35"/>
+    <mergeCell ref="R40:R41"/>
+    <mergeCell ref="AK46:AK47"/>
+    <mergeCell ref="AH40:AH41"/>
+    <mergeCell ref="W40:W41"/>
+    <mergeCell ref="AA40:AA41"/>
+    <mergeCell ref="AI4:AI5"/>
+    <mergeCell ref="AJ4:AJ5"/>
+    <mergeCell ref="AK4:AK5"/>
+    <mergeCell ref="AL4:AL5"/>
+    <mergeCell ref="AM4:AM5"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="X22:X23"/>
+    <mergeCell ref="Y22:Y23"/>
+    <mergeCell ref="Z22:Z23"/>
+    <mergeCell ref="AB22:AB23"/>
+    <mergeCell ref="AC22:AC23"/>
+    <mergeCell ref="AD22:AD23"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="S16:S17"/>
+    <mergeCell ref="T16:T17"/>
+    <mergeCell ref="V10:V11"/>
+    <mergeCell ref="AJ10:AJ11"/>
+    <mergeCell ref="AK10:AK11"/>
+    <mergeCell ref="AL10:AL11"/>
+    <mergeCell ref="AM10:AM11"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="AH13:AH14"/>
+    <mergeCell ref="AM46:AM47"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="AI13:AI14"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="AE19:AE20"/>
+    <mergeCell ref="W22:W23"/>
+    <mergeCell ref="W25:W26"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="AL34:AL35"/>
+    <mergeCell ref="Y40:Y41"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>